<commit_message>
Revert "Merge branch 'master' of https://github.com/jhongarciap/Zoologico"
This reverts commit cd8513579c821f116b203feff2990aef46dc625d, reversing
changes made to 85c2f33dd8d6cd140ff27df903594e589adfee25.
</commit_message>
<xml_diff>
--- a/rom/Employees/Employees.xlsx
+++ b/rom/Employees/Employees.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -75,18 +75,6 @@
   <si>
     <t>sjsjs</t>
   </si>
-  <si>
-    <t>hhhhhhhhhhhhhhhhhhhhhhhhhhh</t>
-  </si>
-  <si>
-    <t>hhhhh</t>
-  </si>
-  <si>
-    <t>hhhhhhhhhhhhhhhhhhh</t>
-  </si>
-  <si>
-    <t>hhhhhhhhhhhhhhhhhhhhhhhhhh</t>
-  </si>
 </sst>
 </file>
 
@@ -130,7 +118,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -192,20 +180,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>